<commit_message>
fix the ID conflict issue
</commit_message>
<xml_diff>
--- a/ontology/ontorat input/medical_specialty.xlsx
+++ b/ontology/ontorat input/medical_specialty.xlsx
@@ -192,7 +192,7 @@
     <t>Mother class</t>
   </si>
   <si>
-    <t>http://www.fda.gov/ontologies/cder/Oreg/OREG_0000023</t>
+    <t>http://www.fda.gov/ontologies/cder/OREG_0000023</t>
   </si>
 </sst>
 </file>
@@ -588,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -614,7 +614,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -882,7 +882,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId1" display="http://www.fda.gov/ontologies/cder/Oreg/OREG_0000023"/>
     <hyperlink ref="D3:D20" r:id="rId2" display="http://www.fda.gov/ontologies/cder/Oreg/OREG_0000023"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>